<commit_message>
New data from today.
</commit_message>
<xml_diff>
--- a/NCBS/Buggy Usage in October 2016.xlsx
+++ b/NCBS/Buggy Usage in October 2016.xlsx
@@ -7,6 +7,15 @@
     <sheet state="visible" name="oct2" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="oct3" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="oct4" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="oct5" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="oct6" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="oct7" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="oct8" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="oct9" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="oct10" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="oct11" sheetId="11" r:id="rId13"/>
+    <sheet state="visible" name="oct12" sheetId="12" r:id="rId14"/>
+    <sheet state="visible" name="oct13" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="5">
   <si>
     <t>Time</t>
   </si>
@@ -62,8 +71,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -136,8 +148,53 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="10">
     <tableStyle count="3" pivot="0" name="oct4-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct6-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct5-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct8-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct9-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct7-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct10-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct11-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct12-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="oct13-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -147,6 +204,22 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -162,14 +235,133 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C27" displayName="oct4" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C27" displayName="oct4" id="2">
   <tableColumns count="3">
     <tableColumn name="Time" id="1"/>
     <tableColumn name="Stop" id="2"/>
     <tableColumn name="Count" id="3"/>
   </tableColumns>
   <tableStyleInfo name="oct4-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct13" id="10">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct13-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C27" displayName="oct5" id="3">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct5-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct6" id="1">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct6-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct7" id="6">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct7-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct8" id="4">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct8-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct9" id="5">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct9-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct10" id="7">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct10-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct11" id="8">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct11-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C29" displayName="oct12" id="9">
+  <tableColumns count="3">
+    <tableColumn name="Time" id="1"/>
+    <tableColumn name="Stop" id="2"/>
+    <tableColumn name="Count" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="oct12-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -479,6 +671,1294 @@
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1410,4 +2890,1604 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>745.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>800.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>830.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>845.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>900.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>915.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>930.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>945.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1030.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1045.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1115.0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1130.0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1300.0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1345.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1400.0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>1430.0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>1500.0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1530.0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>1800.0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>1815.0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>1830.0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>1845.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>1900.0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>1915.0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>2015.0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>